<commit_message>
Add arrows functional to edit page
</commit_message>
<xml_diff>
--- a/converter/src/test/resources/from.xlsx
+++ b/converter/src/test/resources/from.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\kotlin\AlfaConverter\converter\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4397533-34EB-4A71-8E61-18701A9BCBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB9B558-E6F2-46E4-AEEE-329871B64896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12255" yWindow="1860" windowWidth="15525" windowHeight="10965" xr2:uid="{4FFCCFEC-BF92-4A12-94D8-B011486D6CEA}"/>
+    <workbookView xWindow="8895" yWindow="2145" windowWidth="15525" windowHeight="10965" xr2:uid="{4FFCCFEC-BF92-4A12-94D8-B011486D6CEA}"/>
   </bookViews>
   <sheets>
     <sheet name="исходный формат" sheetId="2" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF1500AA-4EF8-4E68-9C39-0CBF91E29FFA}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>